<commit_message>
Getting SEM1.1 to work with Gurobi8 and cvxpy-0.4.11
</commit_message>
<xml_diff>
--- a/case_input.xlsx
+++ b/case_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\SEM-1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53631BB7-2F39-4C3E-B541-670D326741ED}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEEE82D-CD13-412A-8448-CBA1CDCE2C64}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25545" windowHeight="14520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25545" windowHeight="14520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1720" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1720" uniqueCount="177">
   <si>
     <t>This file is documentation for the input data format for the case definition file, used as input for the Simple Energy Model v 1.0</t>
   </si>
@@ -563,6 +563,12 @@
   </si>
   <si>
     <t>2013-2015</t>
+  </si>
+  <si>
+    <t>year_test_03</t>
+  </si>
+  <si>
+    <t>base_test</t>
   </si>
 </sst>
 </file>
@@ -6197,8 +6203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAB1EB0-472A-4DD0-9E69-6F84B61B7AD5}">
   <dimension ref="A1:R108"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52:B53"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6407,7 +6413,7 @@
         <v>19</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>69</v>
+        <v>176</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>20</v>
@@ -7180,7 +7186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283F1F5E-6617-4EDE-A41B-EADB501C3C26}">
   <dimension ref="A1:T142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
@@ -12325,8 +12331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AC059B-0733-439F-A0DB-92535856A335}">
   <dimension ref="A1:T118"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12535,7 +12541,7 @@
         <v>19</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
part way done on adding co2 price and natgas_ccs
</commit_message>
<xml_diff>
--- a/case_input.xlsx
+++ b/case_input.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\SEM-1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB0A7F4-2D1E-4A1E-8294-B6660D11DCC2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8490E571-AF32-4A90-9097-ABD2F107115C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25550" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25550" windowHeight="14520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EIAbaseTest" sheetId="19" r:id="rId1"/>
-    <sheet name="EIAbaseTestMonth" sheetId="26" r:id="rId2"/>
-    <sheet name="testyears" sheetId="23" r:id="rId3"/>
-    <sheet name="test_decay" sheetId="25" r:id="rId4"/>
-    <sheet name="testScaling" sheetId="20" r:id="rId5"/>
-    <sheet name="baseScaling" sheetId="21" r:id="rId6"/>
-    <sheet name="nukeStorScaling" sheetId="22" r:id="rId7"/>
-    <sheet name="PGP storage decay test" sheetId="18" r:id="rId8"/>
+    <sheet name="carbon_cost_test" sheetId="27" r:id="rId2"/>
+    <sheet name="EIAbaseTestMonth" sheetId="26" r:id="rId3"/>
+    <sheet name="testyears" sheetId="23" r:id="rId4"/>
+    <sheet name="test_decay" sheetId="25" r:id="rId5"/>
+    <sheet name="testScaling" sheetId="20" r:id="rId6"/>
+    <sheet name="baseScaling" sheetId="21" r:id="rId7"/>
+    <sheet name="nukeStorScaling" sheetId="22" r:id="rId8"/>
+    <sheet name="PGP storage decay test" sheetId="18" r:id="rId9"/>
   </sheets>
   <calcPr calcId="179021" calcMode="manual"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="180">
   <si>
     <t>This file is documentation for the input data format for the case definition file, used as input for the Simple Energy Model v 1.0</t>
   </si>
@@ -496,15 +497,94 @@
   </si>
   <si>
     <t>EIAbaseTestMonth</t>
+  </si>
+  <si>
+    <t>FIXED_COST_NATGAS_CCS</t>
+  </si>
+  <si>
+    <t>VAR_COST_NATGAS_CCS</t>
+  </si>
+  <si>
+    <t>kgCO2/kWh dispatched</t>
+  </si>
+  <si>
+    <t>VAR_CO2_SOLAR</t>
+  </si>
+  <si>
+    <t>FIXED_CO2_SOLAR</t>
+  </si>
+  <si>
+    <t>kgCO2/kW capacity</t>
+  </si>
+  <si>
+    <t>CO2_COST * FIXED_CO2_SOLAR is added to fixed cost</t>
+  </si>
+  <si>
+    <t>CO2_COST * VAR_CO2_SOLAR is added to variable cost</t>
+  </si>
+  <si>
+    <t>FIXED_CO2_WIND</t>
+  </si>
+  <si>
+    <t>VAR_CO2_WIND</t>
+  </si>
+  <si>
+    <t>FIXED_CO2_NATGAS</t>
+  </si>
+  <si>
+    <t>VAR_CO2_NATGAS</t>
+  </si>
+  <si>
+    <t>FIXED_CO2_NATGAS_CCS</t>
+  </si>
+  <si>
+    <t>VAR_CO2_NATGAS_CCS</t>
+  </si>
+  <si>
+    <t>FIXED_CO2_NUCLEAR</t>
+  </si>
+  <si>
+    <t>VAR_CO2_NUCLEAR</t>
+  </si>
+  <si>
+    <t>CO2_PRICE</t>
+  </si>
+  <si>
+    <t>$/kgCO2:  CO2 price to be used for fixed and variable co2 emissions</t>
+  </si>
+  <si>
+    <t>CO2_COST * VAR_CO2_SOLAR is added to variable cost, source for natgas is https://en.wikipedia.org/wiki/Life-cycle_greenhouse-gas_emissions_of_energy_sources</t>
+  </si>
+  <si>
+    <t>CO2_COST * VAR_CO2_SOLAR is added to variable cost,source for natgas_ccs is https://en.wikipedia.org/wiki/Life-cycle_greenhouse-gas_emissions_of_energy_sources</t>
+  </si>
+  <si>
+    <t>$/kgCO2:  CO2 price to be used for fixed and variable co2 emissions, default is $100 per tonCO2</t>
+  </si>
+  <si>
+    <t>P0000</t>
+  </si>
+  <si>
+    <t>P0010</t>
+  </si>
+  <si>
+    <t>P0100</t>
+  </si>
+  <si>
+    <t>P1000</t>
+  </si>
+  <si>
+    <t>test_price_co2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1001,7 +1081,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1042,6 +1122,9 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1397,10 +1480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528F748F-2438-463B-BA5E-87C8F32FAD91}">
-  <dimension ref="A1:R112"/>
+  <dimension ref="A1:R127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1791,7 +1874,7 @@
       </c>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>37</v>
       </c>
@@ -1803,7 +1886,7 @@
       </c>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>38</v>
       </c>
@@ -1815,7 +1898,7 @@
       </c>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
         <v>39</v>
       </c>
@@ -1827,7 +1910,7 @@
       </c>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>40</v>
       </c>
@@ -1839,162 +1922,164 @@
       </c>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="5"/>
       <c r="B69" s="12"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B70" s="12">
+        <v>0</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71" s="5"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B70" s="12" t="s">
+      <c r="B72" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" s="5" t="s">
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B71" s="14">
+      <c r="B73" s="14">
         <v>2.4911838084243729E-2</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D73" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" s="5" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B72" s="13">
+      <c r="B74" s="13">
         <f>0.00000001</f>
         <v>1E-8</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D72" s="2"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" s="5"/>
-      <c r="B73" s="12"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B74" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B75" s="14">
-        <v>2.0648572594225215E-2</v>
+        <v>158</v>
+      </c>
+      <c r="B75" s="13">
+        <v>0</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>65</v>
+        <v>159</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
-        <v>84</v>
+        <v>157</v>
       </c>
       <c r="B76" s="13">
-        <v>1.0999999999999999E-8</v>
+        <v>0</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D76" s="2"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="5"/>
       <c r="B77" s="12"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B78" s="14">
-        <v>1.1841887362491711E-2</v>
-      </c>
-      <c r="C78" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B79" s="14">
+        <v>2.0648572594225215E-2</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D78" s="16">
-        <v>2.7271220888813726E-2</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B79" s="14">
-        <v>2.2590009128958689E-2</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D79" s="16">
-        <v>2.9679010772171249E-2</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A80" s="5"/>
-      <c r="B80" s="12"/>
-      <c r="C80" s="2"/>
+      <c r="D79" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B80" s="13">
+        <v>1.0999999999999999E-8</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="D80" s="2"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B81" s="14">
-        <v>6.2433901191501419E-2</v>
+        <v>162</v>
+      </c>
+      <c r="B81" s="13">
+        <v>0</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>65</v>
+        <v>159</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>69</v>
+        <v>160</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B82" s="14">
-        <v>2.5158160216169324E-2</v>
+        <v>163</v>
+      </c>
+      <c r="B82" s="13">
+        <v>0</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D82" s="2"/>
+        <v>156</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="5"/>
@@ -2004,403 +2089,599 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B84" s="12">
-        <f>261*0.08/8760</f>
-        <v>2.3835616438356165E-3</v>
+        <v>95</v>
+      </c>
+      <c r="B84" s="14">
+        <v>1.1841887362491711E-2</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
+      </c>
+      <c r="D84" s="16">
+        <v>2.7271220888813726E-2</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B85" s="12">
-        <v>0</v>
+        <v>85</v>
+      </c>
+      <c r="B85" s="14">
+        <v>2.2590009128958689E-2</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D85" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="D85" s="16">
+        <v>2.9679010772171249E-2</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B86" s="12">
+        <v>164</v>
+      </c>
+      <c r="B86" s="13">
         <v>0</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D86" s="2"/>
+        <v>159</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B87" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
-    </row>
-    <row r="88" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B88" s="12">
-        <f>1.01^(1/(24*365.24/12))-1</f>
-        <v>1.3621726294266168E-5</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>48</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="B87" s="18">
+        <v>0.49</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" s="5"/>
+      <c r="B88" s="12"/>
+      <c r="C88" s="2"/>
       <c r="D88" s="2"/>
-      <c r="E88" s="1" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B89" s="12">
-        <v>6</v>
+        <v>154</v>
+      </c>
+      <c r="B89" s="14">
+        <v>2.7271220888813726E-2</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
+      </c>
+      <c r="D89" s="16">
+        <v>2.7271220888813726E-2</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A90" s="5"/>
-      <c r="B90" s="12"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
+      <c r="A90" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B90" s="14">
+        <v>2.9679010772171249E-2</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D90" s="16">
+        <v>2.9679010772171249E-2</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B91" s="12">
-        <v>2.7397260273972604E-6</v>
+        <v>166</v>
+      </c>
+      <c r="B91" s="13">
+        <v>0</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D91" s="12">
-        <f>0.3*0.08/8760</f>
-        <v>2.7397260273972604E-6</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>76</v>
+        <v>159</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B92" s="12">
-        <f>1100*0.08/8760</f>
-        <v>1.0045662100456621E-2</v>
+        <v>167</v>
+      </c>
+      <c r="B92" s="18">
+        <v>0.17</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>65</v>
+        <v>156</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A93" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B93" s="12">
-        <f>4600*0.08/8760</f>
-        <v>4.2009132420091327E-2</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>77</v>
-      </c>
+      <c r="A93" s="5"/>
+      <c r="B93" s="12"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B94" s="12">
-        <v>0</v>
+        <v>96</v>
+      </c>
+      <c r="B94" s="14">
+        <v>6.2433901191501419E-2</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D94" s="2"/>
+      <c r="D94" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B95" s="12">
+        <v>86</v>
+      </c>
+      <c r="B95" s="14">
+        <v>2.5158160216169324E-2</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B96" s="13">
         <v>0</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D95" s="2"/>
-    </row>
-    <row r="96" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B96" s="12">
-        <v>1.1351367708023474E-6</v>
-      </c>
       <c r="C96" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D96" s="12">
-        <f>1.01^(1/(24*365.24))-1</f>
-        <v>1.1351367708023474E-6</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.35">
+        <v>159</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B97" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
-    </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.35">
+        <v>169</v>
+      </c>
+      <c r="B97" s="13">
+        <v>0</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="5"/>
       <c r="B98" s="12"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B99" s="12">
+        <f>261*0.08/8760</f>
+        <v>2.3835616438356165E-3</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A100" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B100" s="12">
+        <v>0</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D100" s="2"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A101" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B101" s="12">
+        <v>0</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D101" s="2"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A102" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B102" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+    </row>
+    <row r="103" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B103" s="12">
+        <f>1.01^(1/(24*365.24/12))-1</f>
+        <v>1.3621726294266168E-5</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D103" s="2"/>
+      <c r="E103" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A104" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B104" s="12">
+        <v>6</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A105" s="5"/>
+      <c r="B105" s="12"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A106" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B106" s="12">
+        <v>2.7397260273972604E-6</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D106" s="12">
+        <f>0.3*0.08/8760</f>
+        <v>2.7397260273972604E-6</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A107" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B107" s="12">
+        <f>1100*0.08/8760</f>
+        <v>1.0045662100456621E-2</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A108" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B108" s="12">
+        <f>4600*0.08/8760</f>
+        <v>4.2009132420091327E-2</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B109" s="12">
+        <v>0</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D109" s="2"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A110" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B110" s="12">
+        <v>0</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D110" s="2"/>
+    </row>
+    <row r="111" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B111" s="12">
+        <v>1.1351367708023474E-6</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D111" s="12">
+        <f>1.01^(1/(24*365.24))-1</f>
+        <v>1.1351367708023474E-6</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A112" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B112" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A113" s="5"/>
+      <c r="B113" s="12"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A114" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B99" s="12">
+      <c r="B114" s="12">
         <v>10</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C114" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D99" s="2"/>
-    </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="C100" s="10"/>
-    </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="C101" s="2" t="s">
+      <c r="D114" s="2"/>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C115" s="10"/>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C116" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="102" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="3" t="s">
+    <row r="117" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A117" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B102" s="11" t="s">
+      <c r="B117" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C102" s="4"/>
-    </row>
-    <row r="103" spans="1:18" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A103" s="5" t="s">
+      <c r="C117" s="4"/>
+    </row>
+    <row r="118" spans="1:18" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A118" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B118" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C103" s="5" t="s">
+      <c r="C118" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="D118" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E103" s="5" t="s">
+      <c r="E118" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F103" s="5" t="s">
+      <c r="F118" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="G103" s="5" t="s">
+      <c r="G118" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="H103" s="5" t="s">
+      <c r="H118" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="I103" s="5" t="s">
+      <c r="I118" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="J103" s="5" t="s">
+      <c r="J118" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="K103" s="5" t="s">
+      <c r="K118" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="L103" s="5" t="s">
+      <c r="L118" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="M103" s="5" t="s">
+      <c r="M118" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="N103" s="5" t="s">
+      <c r="N118" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="O103" s="5" t="s">
+      <c r="O118" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="P103" s="5" t="s">
+      <c r="P118" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="Q103" s="5" t="s">
+      <c r="Q118" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="R103" s="5" t="s">
+      <c r="R118" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B104" s="1"/>
-    </row>
-    <row r="105" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="15" t="s">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B119" s="1"/>
+    </row>
+    <row r="120" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A120" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="B105" s="15">
+      <c r="B120" s="15">
         <v>0.6</v>
       </c>
-      <c r="C105" s="15">
+      <c r="C120" s="15">
         <v>0.6</v>
       </c>
-      <c r="D105" s="15">
-        <v>1</v>
-      </c>
-      <c r="E105" s="15">
-        <v>1</v>
-      </c>
-      <c r="F105" s="15">
+      <c r="D120" s="15">
+        <v>1</v>
+      </c>
+      <c r="E120" s="15">
+        <v>1</v>
+      </c>
+      <c r="F120" s="15">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G105" s="15">
+      <c r="G120" s="15">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H105" s="15">
+      <c r="H120" s="15">
         <v>0.86666666666666003</v>
       </c>
-      <c r="I105" s="15">
+      <c r="I120" s="15">
         <v>0.86666666666666003</v>
       </c>
-      <c r="J105" s="15">
+      <c r="J120" s="15">
         <v>0.4</v>
       </c>
-      <c r="K105" s="15">
+      <c r="K120" s="15">
         <v>0.4</v>
       </c>
-      <c r="L105" s="15">
+      <c r="L120" s="15">
         <v>0.4</v>
       </c>
-      <c r="M105" s="15">
+      <c r="M120" s="15">
         <v>0.2</v>
       </c>
-      <c r="N105" s="15">
+      <c r="N120" s="15">
         <v>0.2</v>
       </c>
-      <c r="O105" s="15">
+      <c r="O120" s="15">
         <v>0.2</v>
       </c>
-      <c r="P105" s="15">
+      <c r="P120" s="15">
         <v>0.2</v>
       </c>
-      <c r="Q105" s="15">
+      <c r="Q120" s="15">
         <v>0.2</v>
       </c>
-      <c r="R105" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="8" t="s">
+      <c r="R120" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A121" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B106" s="6">
-        <v>1</v>
-      </c>
-      <c r="C106" s="6">
-        <v>1</v>
-      </c>
-      <c r="D106" s="6">
-        <v>1</v>
-      </c>
-      <c r="E106" s="6">
-        <v>1</v>
-      </c>
-      <c r="F106" s="6">
-        <v>1</v>
-      </c>
-      <c r="G106" s="6">
-        <v>1</v>
-      </c>
-      <c r="H106" s="6">
-        <v>1</v>
-      </c>
-      <c r="I106" s="6">
-        <v>1</v>
-      </c>
-      <c r="J106" s="6">
-        <v>1</v>
-      </c>
-      <c r="K106" s="6">
-        <v>1</v>
-      </c>
-      <c r="L106" s="6">
-        <v>1</v>
-      </c>
-      <c r="M106" s="6">
-        <v>1</v>
-      </c>
-      <c r="N106" s="6">
-        <v>1</v>
-      </c>
-      <c r="O106" s="6">
-        <v>1</v>
-      </c>
-      <c r="P106" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q106" s="6">
-        <v>1</v>
-      </c>
-      <c r="R106" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="3" t="s">
+      <c r="B121" s="6">
+        <v>1</v>
+      </c>
+      <c r="C121" s="6">
+        <v>1</v>
+      </c>
+      <c r="D121" s="6">
+        <v>1</v>
+      </c>
+      <c r="E121" s="6">
+        <v>1</v>
+      </c>
+      <c r="F121" s="6">
+        <v>1</v>
+      </c>
+      <c r="G121" s="6">
+        <v>1</v>
+      </c>
+      <c r="H121" s="6">
+        <v>1</v>
+      </c>
+      <c r="I121" s="6">
+        <v>1</v>
+      </c>
+      <c r="J121" s="6">
+        <v>1</v>
+      </c>
+      <c r="K121" s="6">
+        <v>1</v>
+      </c>
+      <c r="L121" s="6">
+        <v>1</v>
+      </c>
+      <c r="M121" s="6">
+        <v>1</v>
+      </c>
+      <c r="N121" s="6">
+        <v>1</v>
+      </c>
+      <c r="O121" s="6">
+        <v>1</v>
+      </c>
+      <c r="P121" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q121" s="6">
+        <v>1</v>
+      </c>
+      <c r="R121" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A123" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B108" s="11"/>
-    </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A112" s="1" t="s">
+      <c r="B123" s="11"/>
+    </row>
+    <row r="127" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A127" s="1" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2411,6 +2692,1091 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790C49B8-3B14-4EAF-B724-8E52EEBD60DB}">
+  <dimension ref="A1:E129"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="36" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="16.54296875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="10"/>
+    </row>
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10"/>
+    </row>
+    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="10"/>
+    </row>
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="10"/>
+    </row>
+    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="10"/>
+    </row>
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="10"/>
+    </row>
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="10"/>
+    </row>
+    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="10"/>
+    </row>
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="10"/>
+    </row>
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="10"/>
+    </row>
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="10"/>
+    </row>
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="10"/>
+    </row>
+    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="10"/>
+    </row>
+    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="10"/>
+    </row>
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="10"/>
+    </row>
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="10"/>
+    </row>
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="10"/>
+    </row>
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="10"/>
+    </row>
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="10"/>
+    </row>
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="10"/>
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="10"/>
+    </row>
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="10"/>
+    </row>
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="10"/>
+    </row>
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="10"/>
+    </row>
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="10"/>
+    </row>
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="10"/>
+    </row>
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="10"/>
+    </row>
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="10"/>
+    </row>
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="10"/>
+    </row>
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="10"/>
+    </row>
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="10"/>
+    </row>
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="10"/>
+    </row>
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="10"/>
+    </row>
+    <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="10"/>
+    </row>
+    <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="10"/>
+    </row>
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="10"/>
+    </row>
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="10"/>
+    </row>
+    <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="5"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B49" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C53" s="4"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="13">
+        <v>1000000000000</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="13">
+        <v>1000000000000</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="5"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="2"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C58" s="2"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B59" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" s="5"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B61" s="12">
+        <v>2015</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B62" s="12">
+        <v>1</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" s="12">
+        <v>1</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B64" s="12">
+        <v>1</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B65" s="12">
+        <v>2015</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B66" s="12">
+        <v>12</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B67" s="12">
+        <v>31</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B68" s="12">
+        <v>24</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" s="5"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B70" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71" s="5"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B73" s="14">
+        <v>2.4911838084243729E-2</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B74" s="13">
+        <f>0.00000001</f>
+        <v>1E-8</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B75" s="13">
+        <v>0</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B76" s="13">
+        <v>0</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77" s="5"/>
+      <c r="B77" s="12"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B79" s="14">
+        <v>2.0648572594225215E-2</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B80" s="13">
+        <v>1.0999999999999999E-8</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B81" s="13">
+        <v>0</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B82" s="13">
+        <v>0</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" s="5"/>
+      <c r="B83" s="12"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B84" s="14">
+        <v>1.1841887362491711E-2</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D84" s="16">
+        <v>2.7271220888813726E-2</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85" s="14">
+        <v>2.2590009128958689E-2</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D85" s="16">
+        <v>2.9679010772171249E-2</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B86" s="13">
+        <v>0</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B87" s="18">
+        <v>0.49</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" s="5"/>
+      <c r="B88" s="12"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B89" s="14">
+        <v>2.7271220888813726E-2</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D89" s="16">
+        <v>2.7271220888813726E-2</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B90" s="14">
+        <v>2.9679010772171249E-2</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D90" s="16">
+        <v>2.9679010772171249E-2</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B91" s="13">
+        <v>0</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B92" s="18">
+        <v>0.17</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" s="5"/>
+      <c r="B93" s="12"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B94" s="14">
+        <v>6.2433901191501419E-2</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B95" s="14">
+        <v>2.5158160216169324E-2</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B96" s="13">
+        <v>0</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B97" s="13">
+        <v>0</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A98" s="5"/>
+      <c r="B98" s="12"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A99" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B99" s="12">
+        <f>261*0.08/8760</f>
+        <v>2.3835616438356165E-3</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A100" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B100" s="12">
+        <v>0</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D100" s="2"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A101" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B101" s="12">
+        <v>0</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D101" s="2"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A102" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B102" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+    </row>
+    <row r="103" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B103" s="12">
+        <f>1.01^(1/(24*365.24/12))-1</f>
+        <v>1.3621726294266168E-5</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D103" s="2"/>
+      <c r="E103" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A104" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B104" s="12">
+        <v>6</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A105" s="5"/>
+      <c r="B105" s="12"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A106" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B106" s="12">
+        <v>2.7397260273972604E-6</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D106" s="12">
+        <f>0.3*0.08/8760</f>
+        <v>2.7397260273972604E-6</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A107" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B107" s="12">
+        <f>1100*0.08/8760</f>
+        <v>1.0045662100456621E-2</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A108" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B108" s="12">
+        <f>4600*0.08/8760</f>
+        <v>4.2009132420091327E-2</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B109" s="12">
+        <v>0</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D109" s="2"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A110" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B110" s="12">
+        <v>0</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D110" s="2"/>
+    </row>
+    <row r="111" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B111" s="12">
+        <v>1.1351367708023474E-6</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D111" s="12">
+        <f>1.01^(1/(24*365.24))-1</f>
+        <v>1.1351367708023474E-6</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A112" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B112" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A113" s="5"/>
+      <c r="B113" s="12"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A114" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B114" s="12">
+        <v>10</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D114" s="2"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C115" s="10"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C116" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A117" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B117" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C117" s="4"/>
+    </row>
+    <row r="118" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A118" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B119" s="1"/>
+    </row>
+    <row r="120" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A120" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="B120" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A121" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B121" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A122" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B122" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A123" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B123" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A125" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B125" s="11"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A129" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550DDC27-0C20-441D-A7BC-B4E9F459614A}">
   <dimension ref="A1:R112"/>
   <sheetViews>
@@ -3425,7 +4791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1CA55F3-71CF-4790-ABCB-757487BDCD56}">
   <dimension ref="A1:T120"/>
   <sheetViews>
@@ -4976,7 +6342,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC1A31D-6BD7-4871-811D-118FFE6482B3}">
   <dimension ref="A1:V114"/>
   <sheetViews>
@@ -6193,7 +7559,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7EB0C2-FE99-434C-ADBB-D79DBB252CC7}">
   <dimension ref="A1:T116"/>
   <sheetViews>
@@ -7474,7 +8840,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F36335C-F191-4ED6-89FF-CFA62346621A}">
   <dimension ref="A1:T116"/>
   <sheetViews>
@@ -8755,7 +10121,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515BF5ED-661D-4D09-9F77-3E237FF024FA}">
   <dimension ref="A1:T116"/>
   <sheetViews>
@@ -10036,7 +11402,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D315A23C-713E-4F09-9EE7-90C0F3AF5059}">
   <dimension ref="A1:S112"/>
   <sheetViews>

</xml_diff>